<commit_message>
Updates code and adds new data sources. The code now loops over 4 versions (0,1,2,9) where 9 is EGY MoPED. Evelyn's original version is still there as V1 for reference. The graphs file has three versions, the main on (V2), the one use for Egypt where LGBT is replaced with women's literacty (EGYlbgt) and one (hardcoding) where I modified much of the initial code to be able to compute MENA averages.
</commit_message>
<xml_diff>
--- a/Benchmarking/Benchmarking Variables_V1205.xlsx
+++ b/Benchmarking/Benchmarking Variables_V1205.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eves/Dropbox/MENA/Data/Benchmarking/MENA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/grossitti_worldbank_org/Documents/MENA/terridev_GSG/Benchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB16818C-CF34-2441-A871-A995BE016522}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AB16818C-CF34-2441-A871-A995BE016522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F905E0A0-DB07-4C70-A318-04DAE3F7B561}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="460" windowWidth="22540" windowHeight="15120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparative results " sheetId="3" state="hidden" r:id="rId1"/>
     <sheet name="Versions" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1138,6 +1146,9 @@
     <xf numFmtId="0" fontId="7" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1169,9 +1180,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1474,18 +1482,18 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="36.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.875" customWidth="1"/>
+    <col min="4" max="4" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="25.125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="22.625" customWidth="1"/>
     <col min="8" max="8" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1504,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1530,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>2</v>
@@ -1544,7 +1552,7 @@
       </c>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="36" t="s">
         <v>3</v>
@@ -1565,7 +1573,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>4</v>
@@ -1584,7 +1592,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>5</v>
@@ -1603,7 +1611,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="11" t="s">
         <v>6</v>
@@ -1624,13 +1632,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="1"/>
       <c r="E9" s="27"/>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
@@ -1654,7 +1662,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="10" t="s">
         <v>9</v>
@@ -1675,7 +1683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
         <v>10</v>
@@ -1693,7 +1701,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -1712,7 +1720,7 @@
       </c>
       <c r="G13" s="35"/>
     </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="10" t="s">
         <v>12</v>
@@ -1733,7 +1741,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="10" t="s">
         <v>13</v>
@@ -1754,7 +1762,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="10" t="s">
         <v>14</v>
@@ -1775,7 +1783,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="10" t="s">
         <v>15</v>
@@ -1799,7 +1807,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="10" t="s">
         <v>16</v>
@@ -1820,7 +1828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="14" t="s">
         <v>17</v>
@@ -1839,7 +1847,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
         <v>18</v>
@@ -1856,7 +1864,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="14" t="s">
         <v>19</v>
@@ -1873,7 +1881,7 @@
       </c>
       <c r="G21" s="31"/>
     </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="11" t="s">
         <v>20</v>
@@ -1892,7 +1900,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>21</v>
       </c>
@@ -1918,7 +1926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="18" t="s">
         <v>23</v>
@@ -1939,7 +1947,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="10" t="s">
         <v>24</v>
@@ -1960,7 +1968,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="10" t="s">
         <v>25</v>
@@ -1981,7 +1989,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="10" t="s">
         <v>26</v>
@@ -2000,7 +2008,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="10" t="s">
         <v>27</v>
@@ -2024,7 +2032,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="10" t="s">
         <v>28</v>
@@ -2046,7 +2054,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="20" t="s">
         <v>29</v>
@@ -2065,7 +2073,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>30</v>
       </c>
@@ -2086,7 +2094,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
       <c r="B32" s="10" t="s">
         <v>32</v>
@@ -2105,7 +2113,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="10" t="s">
         <v>33</v>
@@ -2126,7 +2134,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="18" t="s">
         <v>34</v>
@@ -2150,7 +2158,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="18" t="s">
         <v>35</v>
@@ -2174,7 +2182,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="18" t="s">
         <v>36</v>
@@ -2201,7 +2209,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="24" t="s">
         <v>37</v>
@@ -2233,36 +2241,36 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="33.125" customWidth="1"/>
     <col min="4" max="4" width="42.5" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="79" t="s">
+    <row r="1" spans="1:7" ht="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="80" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-    </row>
-    <row r="3" spans="1:7" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="90" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+    </row>
+    <row r="3" spans="1:7" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="79" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="48" t="s">
         <v>115</v>
       </c>
@@ -2279,11 +2287,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="81" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="46">
@@ -2302,11 +2310,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="81"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="47">
         <v>2017</v>
       </c>
@@ -2323,11 +2331,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="81"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="47">
         <v>2019</v>
       </c>
@@ -2344,11 +2352,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="81"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="47" t="s">
         <v>158</v>
       </c>
@@ -2365,11 +2373,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="81"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="47" t="s">
         <v>159</v>
       </c>
@@ -2386,11 +2394,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="47">
         <v>2014</v>
       </c>
@@ -2407,11 +2415,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="85" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="51" t="s">
@@ -2430,11 +2438,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="85"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="52">
         <v>2018</v>
       </c>
@@ -2451,11 +2459,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="85"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="52">
         <v>2017</v>
       </c>
@@ -2472,11 +2480,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="85"/>
+      <c r="B14" s="86"/>
       <c r="C14" s="52">
         <v>2017</v>
       </c>
@@ -2493,11 +2501,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="85"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="52">
         <v>2017</v>
       </c>
@@ -2514,11 +2522,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="52" t="s">
         <v>124</v>
       </c>
@@ -2535,11 +2543,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="85"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="52" t="s">
         <v>124</v>
       </c>
@@ -2556,11 +2564,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="85"/>
+      <c r="B18" s="86"/>
       <c r="C18" s="52">
         <v>2018</v>
       </c>
@@ -2577,11 +2585,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="85"/>
+      <c r="B19" s="86"/>
       <c r="C19" s="52" t="s">
         <v>152</v>
       </c>
@@ -2598,11 +2606,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="85"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="52" t="s">
         <v>126</v>
       </c>
@@ -2619,11 +2627,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21" s="85"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="52">
         <v>2020</v>
       </c>
@@ -2640,11 +2648,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" s="85"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="52" t="s">
         <v>153</v>
       </c>
@@ -2661,11 +2669,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="85"/>
+      <c r="B23" s="86"/>
       <c r="C23" s="52" t="s">
         <v>153</v>
       </c>
@@ -2682,11 +2690,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="85"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="59">
         <v>2020</v>
       </c>
@@ -2703,11 +2711,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="86"/>
+      <c r="B25" s="87"/>
       <c r="C25" s="60">
         <v>2020</v>
       </c>
@@ -2724,11 +2732,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="88" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="62">
@@ -2747,11 +2755,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
-      <c r="B27" s="88"/>
+      <c r="B27" s="89"/>
       <c r="C27" s="62">
         <v>2016</v>
       </c>
@@ -2768,11 +2776,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
-      <c r="B28" s="88"/>
+      <c r="B28" s="89"/>
       <c r="C28" s="62" t="s">
         <v>134</v>
       </c>
@@ -2792,11 +2800,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
-      <c r="B29" s="88"/>
+      <c r="B29" s="89"/>
       <c r="C29" s="62">
         <v>2015</v>
       </c>
@@ -2813,11 +2821,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
-      <c r="B30" s="88"/>
+      <c r="B30" s="89"/>
       <c r="C30" s="62">
         <v>2014</v>
       </c>
@@ -2834,11 +2842,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
-      <c r="B31" s="88"/>
+      <c r="B31" s="89"/>
       <c r="C31" s="62" t="s">
         <v>157</v>
       </c>
@@ -2855,11 +2863,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
-      <c r="B32" s="88"/>
+      <c r="B32" s="89"/>
       <c r="C32" s="62">
         <v>2020</v>
       </c>
@@ -2876,11 +2884,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
-      <c r="B33" s="88"/>
+      <c r="B33" s="89"/>
       <c r="C33" s="62" t="s">
         <v>156</v>
       </c>
@@ -2897,11 +2905,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
-      <c r="B34" s="88"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="62" t="s">
         <v>163</v>
       </c>
@@ -2918,11 +2926,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
-      <c r="B35" s="88"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="62">
         <v>2020</v>
       </c>
@@ -2939,11 +2947,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="89"/>
       <c r="C36" s="62">
         <v>2020</v>
       </c>
@@ -2960,11 +2968,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
-      <c r="B37" s="88"/>
+      <c r="B37" s="89"/>
       <c r="C37" s="62">
         <v>2020</v>
       </c>
@@ -2981,11 +2989,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>34</v>
       </c>
-      <c r="B38" s="89"/>
+      <c r="B38" s="90"/>
       <c r="C38" s="65">
         <v>2016</v>
       </c>
@@ -3002,11 +3010,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
-      <c r="B39" s="82" t="s">
+      <c r="B39" s="83" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="67">
@@ -3025,11 +3033,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="83"/>
       <c r="C40" s="67">
         <v>2016</v>
       </c>
@@ -3046,11 +3054,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
-      <c r="B41" s="82"/>
+      <c r="B41" s="83"/>
       <c r="C41" s="67">
         <v>2012</v>
       </c>
@@ -3067,11 +3075,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
-      <c r="B42" s="82"/>
+      <c r="B42" s="83"/>
       <c r="C42" s="67">
         <v>2018</v>
       </c>
@@ -3088,11 +3096,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="83"/>
       <c r="C43" s="67">
         <v>2018</v>
       </c>
@@ -3109,11 +3117,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
-      <c r="B44" s="82"/>
+      <c r="B44" s="83"/>
       <c r="C44" s="67">
         <v>2018</v>
       </c>
@@ -3130,11 +3138,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41</v>
       </c>
-      <c r="B45" s="82"/>
+      <c r="B45" s="83"/>
       <c r="C45" s="67" t="s">
         <v>154</v>
       </c>
@@ -3151,11 +3159,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
-      <c r="B46" s="82"/>
+      <c r="B46" s="83"/>
       <c r="C46" s="67">
         <v>2017</v>
       </c>
@@ -3172,11 +3180,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>43</v>
       </c>
-      <c r="B47" s="82"/>
+      <c r="B47" s="83"/>
       <c r="C47" s="67" t="s">
         <v>160</v>
       </c>
@@ -3193,11 +3201,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>44</v>
       </c>
-      <c r="B48" s="82"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="67" t="s">
         <v>152</v>
       </c>
@@ -3214,11 +3222,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>45</v>
       </c>
-      <c r="B49" s="82"/>
+      <c r="B49" s="83"/>
       <c r="C49" s="67" t="s">
         <v>161</v>
       </c>
@@ -3235,11 +3243,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>46</v>
       </c>
-      <c r="B50" s="83"/>
+      <c r="B50" s="84"/>
       <c r="C50" s="70"/>
       <c r="D50" s="71" t="s">
         <v>102</v>
@@ -3254,7 +3262,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D51" s="5"/>
     </row>
   </sheetData>

</xml_diff>